<commit_message>
plumbing data showing now
-changes in quries in prisma
-table elemts change accroding to requirements.

-this was extremly frustrated process
-have develop input method to plumning fitting
-have to build slon & anton with separated elemets

-dected major table change in price & brand tables
-brand elemnt have to be on price table
-its extremly hard one. but have to do it.
</commit_message>
<xml_diff>
--- a/backend/data/plumData/plumTableData/plumInfoall.xlsx
+++ b/backend/data/plumData/plumTableData/plumInfoall.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\projects\MY_PROJECTS\material-database\data\plumData\plumTableData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\projects\MY_PROJECTS\web_application\backend\data\plumData\plumTableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3CFCE8-4D4C-469F-8B0C-44B74BA5DFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3E5B23-5340-4BF6-B095-CE950AEA122F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{A0BBE691-86F4-4964-8F22-F4C94C854054}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="14745" windowHeight="7815" firstSheet="4" activeTab="4" xr2:uid="{A0BBE691-86F4-4964-8F22-F4C94C854054}"/>
   </bookViews>
   <sheets>
     <sheet name="size" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="201">
   <si>
     <t>20mm</t>
   </si>
@@ -643,6 +643,30 @@
   </si>
   <si>
     <t>plumClass</t>
+  </si>
+  <si>
+    <t>75mm x 32mm</t>
+  </si>
+  <si>
+    <t>75mm x 40mm</t>
+  </si>
+  <si>
+    <t>75mm x 50mm</t>
+  </si>
+  <si>
+    <t>75mm x 63mm</t>
+  </si>
+  <si>
+    <t>2  1/2" x 1"</t>
+  </si>
+  <si>
+    <t>2  1/2" x 1 1/4"</t>
+  </si>
+  <si>
+    <t>2  1/2" x 1 1/2"</t>
+  </si>
+  <si>
+    <t>2  1/2" x 2"</t>
   </si>
 </sst>
 </file>
@@ -1006,10 +1030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1537CBF8-F71A-411B-9DB0-DEF6645F17DF}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,12 +1084,12 @@
         <v>"1/2\""</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G33" si="0">_xlfn.CONCAT( "(",D2,", ", F2,")")</f>
+        <f t="shared" ref="G2:G37" si="0">_xlfn.CONCAT( "(",D2,", ", F2,")")</f>
         <v>("20mm", "1/2\"")</v>
       </c>
       <c r="H2" t="str" cm="1">
-        <f t="array" ref="H2">_xlfn.CONCAT("INSERT INTO plumsizes (plumSizeImperial,plumSizeMetric) VALUES",(TRANSPOSE(G2:G34)&amp;","))</f>
-        <v>INSERT INTO plumsizes (plumSizeImperial,plumSizeMetric) VALUES("20mm", "1/2\""),("25mm", "3/4\""),("32mm", "1\""),("40mm", "1 1/4\""),("50mm", "1 1/2\""),("63mm", "2\""),("75mm", "2 1/2\""),("90mm", "3\""),("110mm", "4\""),("25mm x 20mm", "3/4\" x 1/2\""),("32mm x 20mm", "1\" x 1/2\""),("32mm x 25mm", "1\" x 3/4\""),("40mm x 20mm", "1 1/4\" x 1/2\""),("40mm x 25mm", "1 1/4\" x 3/4\""),("40mm x 32mm", "1 1/4\" x 1\""),("50mmx 20mm", "1 1/2\" x 1/2\""),("50mm x 25mm", "1 1/2\" x 3/4\""),("50mm x 32mm", "1 1/2\" x 1\""),("50mm x 40mm", "1 1/2\" x 1 1/4\""),("63mm x 20mm", "2\" x 1/2\""),("63mm x 25mm", "2\" x 3/4\""),("63mm x 32mm", "2\" x 1\""),("63mm x 40mm", "2\" x 1 1/4\""),("63mm x 50mm", "2\" x 1 1/2\""),("90mm x 40mm", "3\" x 1 1/4\""),("90mm x 50mm", "3\" x 1 1/2\""),("90mm x 63mm", "3\" x 2\""),("90mm x 75mm", "3\" x 2 1/2\""),("110mm x 50mm", "4\" x 1 1/2\""),("110mm x 63mm", "4\" x 2\""),("110mm x 75mm", "4\" x 2 1/2\""),("110mm x 90mm", "4\" x 3\""),("160mm", "6\""),</v>
+        <f t="array" ref="H2">_xlfn.CONCAT("INSERT INTO plumsizes (plumSizeImperial,plumSizeMetric) VALUES",(TRANSPOSE(G2:G38)&amp;","))</f>
+        <v>INSERT INTO plumsizes (plumSizeImperial,plumSizeMetric) VALUES("20mm", "1/2\""),("25mm", "3/4\""),("32mm", "1\""),("40mm", "1 1/4\""),("50mm", "1 1/2\""),("63mm", "2\""),("75mm", "2 1/2\""),("90mm", "3\""),("110mm", "4\""),("25mm x 20mm", "3/4\" x 1/2\""),("32mm x 20mm", "1\" x 1/2\""),("32mm x 25mm", "1\" x 3/4\""),("40mm x 20mm", "1 1/4\" x 1/2\""),("40mm x 25mm", "1 1/4\" x 3/4\""),("40mm x 32mm", "1 1/4\" x 1\""),("50mmx 20mm", "1 1/2\" x 1/2\""),("50mm x 25mm", "1 1/2\" x 3/4\""),("50mm x 32mm", "1 1/2\" x 1\""),("50mm x 40mm", "1 1/2\" x 1 1/4\""),("63mm x 20mm", "2\" x 1/2\""),("63mm x 25mm", "2\" x 3/4\""),("63mm x 32mm", "2\" x 1\""),("63mm x 40mm", "2\" x 1 1/4\""),("63mm x 50mm", "2\" x 1 1/2\""),("75mm x 32mm", "2\" x 1 1/2\""),("75mm x 40mm", "2\" x 1 1/2\""),("75mm x 50mm", "2\" x 1 1/2\""),("75mm x 63mm", "2\" x 1 1/2\""),("90mm x 40mm", "3\" x 1 1/4\""),("90mm x 50mm", "3\" x 1 1/2\""),("90mm x 63mm", "3\" x 2\""),("90mm x 75mm", "3\" x 2 1/2\""),("110mm x 50mm", "4\" x 1 1/2\""),("110mm x 63mm", "4\" x 2\""),("110mm x 75mm", "4\" x 2 1/2\""),("110mm x 90mm", "4\" x 3\""),("160mm", "6\""),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1079,14 +1103,14 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="str">
-        <f t="shared" ref="D3:D33" si="1">_xlfn.CONCAT(""""&amp;B3&amp;"""")</f>
+        <f t="shared" ref="D3:D37" si="1">_xlfn.CONCAT(""""&amp;B3&amp;"""")</f>
         <v>"25mm"</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>141</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f t="shared" ref="F3:F33" si="2">_xlfn.CONCAT(""""&amp;E3&amp;"""")</f>
+        <f t="shared" ref="F3:F37" si="2">_xlfn.CONCAT(""""&amp;E3&amp;"""")</f>
         <v>"3/4\""</v>
       </c>
       <c r="G3" t="str">
@@ -1671,25 +1695,25 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>193</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>49</v>
+        <v>197</v>
       </c>
       <c r="D26" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>"90mm x 40mm"</v>
+        <v>"75mm x 32mm"</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"3\" x 1 1/4\""</v>
+        <v>"2\" x 1 1/2\""</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>("90mm x 40mm", "3\" x 1 1/4\"")</v>
+        <v>("75mm x 32mm", "2\" x 1 1/2\"")</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1697,25 +1721,25 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>50</v>
+        <v>194</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>51</v>
+        <v>198</v>
       </c>
       <c r="D27" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>"90mm x 50mm"</v>
+        <v>"75mm x 40mm"</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"3\" x 1 1/2\""</v>
+        <v>"2\" x 1 1/2\""</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>("90mm x 50mm", "3\" x 1 1/2\"")</v>
+        <v>("75mm x 40mm", "2\" x 1 1/2\"")</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1723,25 +1747,25 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>52</v>
+        <v>195</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>53</v>
+        <v>199</v>
       </c>
       <c r="D28" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>"90mm x 63mm"</v>
+        <v>"75mm x 50mm"</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"3\" x 2\""</v>
+        <v>"2\" x 1 1/2\""</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>("90mm x 63mm", "3\" x 2\"")</v>
+        <v>("75mm x 50mm", "2\" x 1 1/2\"")</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1749,25 +1773,25 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>54</v>
+        <v>196</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>55</v>
+        <v>200</v>
       </c>
       <c r="D29" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>"90mm x 75mm"</v>
+        <v>"75mm x 63mm"</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"3\" x 2 1/2\""</v>
+        <v>"2\" x 1 1/2\""</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>("90mm x 75mm", "3\" x 2 1/2\"")</v>
+        <v>("75mm x 63mm", "2\" x 1 1/2\"")</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1775,25 +1799,25 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D30" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>"110mm x 50mm"</v>
+        <v>"90mm x 40mm"</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"4\" x 1 1/2\""</v>
+        <v>"3\" x 1 1/4\""</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v>("110mm x 50mm", "4\" x 1 1/2\"")</v>
+        <v>("90mm x 40mm", "3\" x 1 1/4\"")</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1801,25 +1825,25 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D31" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>"110mm x 63mm"</v>
+        <v>"90mm x 50mm"</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"4\" x 2\""</v>
+        <v>"3\" x 1 1/2\""</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v>("110mm x 63mm", "4\" x 2\"")</v>
+        <v>("90mm x 50mm", "3\" x 1 1/2\"")</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1827,25 +1851,25 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D32" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>"110mm x 75mm"</v>
+        <v>"90mm x 63mm"</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"4\" x 2 1/2\""</v>
+        <v>"3\" x 2\""</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
-        <v>("110mm x 75mm", "4\" x 2 1/2\"")</v>
+        <v>("90mm x 63mm", "3\" x 2\"")</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1853,25 +1877,25 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D33" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>"110mm x 90mm"</v>
+        <v>"90mm x 75mm"</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"4\" x 3\""</v>
+        <v>"3\" x 2 1/2\""</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
-        <v>("110mm x 90mm", "4\" x 3\"")</v>
+        <v>("90mm x 75mm", "3\" x 2 1/2\"")</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1879,29 +1903,135 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>"110mm x 50mm"</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F34" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>"4\" x 1 1/2\""</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>("110mm x 50mm", "4\" x 1 1/2\"")</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>"110mm x 63mm"</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F35" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>"4\" x 2\""</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>("110mm x 63mm", "4\" x 2\"")</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>"110mm x 75mm"</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F36" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>"4\" x 2 1/2\""</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>("110mm x 75mm", "4\" x 2 1/2\"")</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>"110mm x 90mm"</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F37" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>"4\" x 3\""</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v>("110mm x 90mm", "4\" x 3\"")</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D34" s="1" t="str">
-        <f t="shared" ref="D34" si="3">_xlfn.CONCAT(""""&amp;B34&amp;"""")</f>
+      <c r="D38" s="1" t="str">
+        <f t="shared" ref="D38" si="3">_xlfn.CONCAT(""""&amp;B38&amp;"""")</f>
         <v>"160mm"</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F34" s="1" t="str">
-        <f t="shared" ref="F34" si="4">_xlfn.CONCAT(""""&amp;E34&amp;"""")</f>
+      <c r="F38" s="1" t="str">
+        <f t="shared" ref="F38" si="4">_xlfn.CONCAT(""""&amp;E38&amp;"""")</f>
         <v>"6\""</v>
       </c>
-      <c r="G34" t="str">
-        <f t="shared" ref="G34" si="5">_xlfn.CONCAT( "(",D34,", ", F34,")")</f>
+      <c r="G38" t="str">
+        <f t="shared" ref="G38" si="5">_xlfn.CONCAT( "(",D38,", ", F38,")")</f>
         <v>("160mm", "6\"")</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1910,7 +2040,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1958,8 +2088,8 @@
         <v>("uPVC PNT 14", "SLS 147:2013 ")</v>
       </c>
       <c r="G2" t="str" cm="1">
-        <f t="array" ref="G2">_xlfn.CONCAT("INSERT INTO plumClass (plumClass,plumStandard) VALUES",(TRANSPOSE(F2:F14)&amp;","))</f>
-        <v>INSERT INTO plumClass (plumClass,plumStandard) VALUES("uPVC PNT 14", "SLS 147:2013 "),("uPVC PNT 14 - Fitting", "SLS 659:2015"),(" uPVC PNT 11", "SLS 147:2013 "),(" uPVC PNT 11 - Fitting", "SLS 659:2015"),(" uPVC PNT 12.5 - Fitting", "SLS 659:2016"),(" uPVC PNT 7", "SLS 147:2013 "),(" uPVC CLASS 4.0 ", "SLS 1325"),(" uPVCCLASS 2.5", "SLS 1325"),("uPVC Drainage - fittings", "SLS 1325"),("uPVC Drainage (special) SS", "SLS 1286"),("Tube Well Pipe SS", "Non-Type"),("Irrigation Pipe SS", "Non-Type"),("CPVC", "IS : 15778"),</v>
+        <f t="array" ref="G2">_xlfn.CONCAT("INSERT INTO plumGrade (plumClass,plumStandard) VALUES",(TRANSPOSE(F2:F14)&amp;","))</f>
+        <v>INSERT INTO plumGrade (plumClass,plumStandard) VALUES("uPVC PNT 14", "SLS 147:2013 "),("uPVC PNT 14 - Fitting", "SLS 659:2015"),(" uPVC PNT 11", "SLS 147:2013 "),(" uPVC PNT 11 - Fitting", "SLS 659:2015"),(" uPVC PNT 12.5 - Fitting", "SLS 659:2016"),(" uPVC PNT 7", "SLS 147:2013 "),(" uPVC CLASS 4.0 ", "SLS 1325"),(" uPVCCLASS 2.5", "SLS 1325"),("uPVC Drainage - fittings", "SLS 1325"),("uPVC Drainage (special) SS", "SLS 1286"),("Tube Well Pipe SS", "Non-Type"),("Irrigation Pipe SS", "Non-Type"),("CPVC", "IS : 15778"),</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1973,15 +2103,15 @@
         <v>108</v>
       </c>
       <c r="D3" s="1" t="str">
-        <f t="shared" ref="D3:D14" si="0">_xlfn.CONCAT(""""&amp;B3&amp;"""")</f>
+        <f>_xlfn.CONCAT(""""&amp;B3&amp;"""")</f>
         <v>"uPVC PNT 14 - Fitting"</v>
       </c>
       <c r="E3" s="1" t="str">
-        <f t="shared" ref="E3:E14" si="1">_xlfn.CONCAT(""""&amp;C3&amp;"""")</f>
+        <f>_xlfn.CONCAT(""""&amp;C3&amp;"""")</f>
         <v>"SLS 659:2015"</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F14" si="2">_xlfn.CONCAT( "(",D3,", ", E3,")")</f>
+        <f t="shared" ref="F3:F14" si="0">_xlfn.CONCAT( "(",D3,", ", E3,")")</f>
         <v>("uPVC PNT 14 - Fitting", "SLS 659:2015")</v>
       </c>
     </row>
@@ -1996,15 +2126,15 @@
         <v>105</v>
       </c>
       <c r="D4" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(""""&amp;B4&amp;"""")</f>
         <v>" uPVC PNT 11"</v>
       </c>
       <c r="E4" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(""""&amp;C4&amp;"""")</f>
         <v>"SLS 147:2013 "</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>(" uPVC PNT 11", "SLS 147:2013 ")</v>
       </c>
     </row>
@@ -2019,15 +2149,15 @@
         <v>108</v>
       </c>
       <c r="D5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(""""&amp;B5&amp;"""")</f>
         <v>" uPVC PNT 11 - Fitting"</v>
       </c>
       <c r="E5" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(""""&amp;C5&amp;"""")</f>
         <v>"SLS 659:2015"</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>(" uPVC PNT 11 - Fitting", "SLS 659:2015")</v>
       </c>
     </row>
@@ -2042,15 +2172,15 @@
         <v>178</v>
       </c>
       <c r="D6" s="1" t="str">
-        <f t="shared" ref="D6" si="3">_xlfn.CONCAT(""""&amp;B6&amp;"""")</f>
+        <f>_xlfn.CONCAT(""""&amp;B6&amp;"""")</f>
         <v>" uPVC PNT 12.5 - Fitting"</v>
       </c>
       <c r="E6" s="1" t="str">
-        <f t="shared" ref="E6" si="4">_xlfn.CONCAT(""""&amp;C6&amp;"""")</f>
+        <f>_xlfn.CONCAT(""""&amp;C6&amp;"""")</f>
         <v>"SLS 659:2016"</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" ref="F6" si="5">_xlfn.CONCAT( "(",D6,", ", E6,")")</f>
+        <f t="shared" ref="F6" si="1">_xlfn.CONCAT( "(",D6,", ", E6,")")</f>
         <v>(" uPVC PNT 12.5 - Fitting", "SLS 659:2016")</v>
       </c>
     </row>
@@ -2065,15 +2195,15 @@
         <v>105</v>
       </c>
       <c r="D7" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(""""&amp;B7&amp;"""")</f>
         <v>" uPVC PNT 7"</v>
       </c>
       <c r="E7" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(""""&amp;C7&amp;"""")</f>
         <v>"SLS 147:2013 "</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>(" uPVC PNT 7", "SLS 147:2013 ")</v>
       </c>
     </row>
@@ -2088,15 +2218,15 @@
         <v>110</v>
       </c>
       <c r="D8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(""""&amp;B8&amp;"""")</f>
         <v>" uPVC CLASS 4.0 "</v>
       </c>
       <c r="E8" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(""""&amp;C8&amp;"""")</f>
         <v>"SLS 1325"</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>(" uPVC CLASS 4.0 ", "SLS 1325")</v>
       </c>
     </row>
@@ -2111,15 +2241,15 @@
         <v>110</v>
       </c>
       <c r="D9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(""""&amp;B9&amp;"""")</f>
         <v>" uPVCCLASS 2.5"</v>
       </c>
       <c r="E9" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(""""&amp;C9&amp;"""")</f>
         <v>"SLS 1325"</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>(" uPVCCLASS 2.5", "SLS 1325")</v>
       </c>
     </row>
@@ -2134,15 +2264,15 @@
         <v>110</v>
       </c>
       <c r="D10" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(""""&amp;B10&amp;"""")</f>
         <v>"uPVC Drainage - fittings"</v>
       </c>
       <c r="E10" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(""""&amp;C10&amp;"""")</f>
         <v>"SLS 1325"</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>("uPVC Drainage - fittings", "SLS 1325")</v>
       </c>
     </row>
@@ -2157,15 +2287,15 @@
         <v>109</v>
       </c>
       <c r="D11" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(""""&amp;B11&amp;"""")</f>
         <v>"uPVC Drainage (special) SS"</v>
       </c>
       <c r="E11" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(""""&amp;C11&amp;"""")</f>
         <v>"SLS 1286"</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>("uPVC Drainage (special) SS", "SLS 1286")</v>
       </c>
     </row>
@@ -2180,15 +2310,15 @@
         <v>113</v>
       </c>
       <c r="D12" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(""""&amp;B12&amp;"""")</f>
         <v>"Tube Well Pipe SS"</v>
       </c>
       <c r="E12" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(""""&amp;C12&amp;"""")</f>
         <v>"Non-Type"</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>("Tube Well Pipe SS", "Non-Type")</v>
       </c>
     </row>
@@ -2203,15 +2333,15 @@
         <v>113</v>
       </c>
       <c r="D13" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(""""&amp;B13&amp;"""")</f>
         <v>"Irrigation Pipe SS"</v>
       </c>
       <c r="E13" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(""""&amp;C13&amp;"""")</f>
         <v>"Non-Type"</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>("Irrigation Pipe SS", "Non-Type")</v>
       </c>
     </row>
@@ -2226,15 +2356,15 @@
         <v>112</v>
       </c>
       <c r="D14" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(""""&amp;B14&amp;"""")</f>
         <v>"CPVC"</v>
       </c>
       <c r="E14" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(""""&amp;C14&amp;"""")</f>
         <v>"IS : 15778"</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>("CPVC", "IS : 15778")</v>
       </c>
     </row>
@@ -2413,8 +2543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD89E6EC-8F15-4548-81F8-F39FFF15A66D}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3277,10 +3407,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F8B51A4-0C2E-4883-BC0A-528D5C113E23}">
-  <dimension ref="A1:H176"/>
+  <dimension ref="A1:H184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3338,8 +3468,8 @@
         <v>(1, 1, 2, 1, 2)</v>
       </c>
       <c r="H2" t="str" cm="1">
-        <f t="array" ref="H2">_xlfn.CONCAT("INSERT INTO plumfittinginfos (plumFittingId,plumBrandId,plumGradeId,plumSizeId,plumTypeId) VALUES",(TRANSPOSE(G2:G176)&amp;","))</f>
-        <v>INSERT INTO plumfittinginfos (plumFittingId,plumBrandId,plumGradeId,plumSizeId,plumTypeId) VALUES(1, 1, 2, 1, 2),(1, 1, 4, 2, 2),(1, 1, 4, 3, 2),(1, 1, 4, 4, 2),(1, 1, 4, 5, 2),(1, 1, 4, 6, 2),(1, 1, 4, 7, 2),(1, 1, 4, 8, 2),(1, 1, 4, 9, 2),(2, 1, 2, 1, 2),(2, 1, 4, 2, 2),(2, 1, 4, 3, 2),(2, 1, 4, 4, 2),(2, 1, 4, 5, 2),(2, 1, 4, 6, 2),(2, 1, 4, 7, 2),(2, 1, 4, 8, 2),(2, 1, 4, 9, 2),(3, 1, 2, 1, 2),(3, 1, 4, 2, 2),(3, 1, 4, 3, 2),(3, 1, 4, 4, 2),(3, 1, 4, 5, 2),(3, 1, 4, 6, 2),(3, 1, 4, 7, 2),(3, 1, 4, 8, 2),(3, 1, 4, 9, 2),(4, 1, 2, 1, 2),(4, 1, 4, 2, 2),(4, 1, 4, 3, 2),(4, 1, 4, 4, 2),(4, 1, 4, 5, 2),(4, 1, 4, 6, 2),(4, 1, 4, 7, 2),(4, 1, 4, 8, 2),(4, 1, 4, 9, 2),(5, 1, 2, 1, 2),(5, 1, 4, 2, 2),(5, 1, 4, 3, 2),(5, 1, 4, 4, 2),(5, 1, 4, 5, 2),(5, 1, 4, 6, 2),(5, 1, 4, 7, 2),(5, 1, 4, 8, 2),(5, 1, 4, 9, 2),(6, 1, 2, 1, 2),(6, 1, 4, 2, 2),(6, 1, 4, 3, 2),(6, 1, 4, 4, 2),(6, 1, 4, 5, 2),(6, 1, 4, 6, 2),(6, 1, 4, 7, 2),(6, 1, 4, 8, 2),(6, 1, 4, 9, 2),(7, 1, 2, 1, 2),(7, 1, 4, 2, 2),(7, 1, 4, 3, 2),(7, 1, 4, 4, 2),(7, 1, 4, 5, 2),(7, 1, 4, 6, 2),(7, 1, 4, 7, 2),(7, 1, 4, 8, 2),(7, 1, 4, 9, 2),(8, 1, 2, 1, 2),(8, 1, 4, 2, 2),(8, 1, 4, 3, 2),(8, 1, 4, 4, 2),(8, 1, 4, 5, 2),(8, 1, 4, 6, 2),(8, 1, 4, 7, 2),(8, 1, 4, 8, 2),(8, 1, 4, 9, 2),(9, 1, 2, 1, 2),(9, 1, 4, 2, 2),(9, 1, 4, 3, 2),(9, 1, 4, 4, 2),(9, 1, 4, 5, 2),(9, 1, 4, 6, 2),(10, 1, 4, 10, 2),(10, 1, 4, 11, 2),(10, 1, 4, 12, 2),(10, 1, 4, 13, 2),(10, 1, 4, 14, 2),(10, 1, 4, 15, 2),(10, 1, 4, 16, 2),(10, 1, 4, 17, 2),(10, 1, 4, 18, 2),(10, 1, 4, 19, 2),(10, 1, 4, 20, 2),(10, 1, 4, 21, 2),(10, 1, 4, 22, 2),(10, 1, 4, 23, 2),(10, 1, 4, 24, 2),(10, 1, 4, 25, 2),(10, 1, 4, 26, 2),(10, 1, 4, 27, 2),(10, 1, 4, 28, 2),(10, 1, 4, 29, 2),(10, 1, 4, 30, 2),(10, 1, 4, 31, 2),(10, 1, 4, 32, 2),(11, 1, 4, 10, 2),(11, 1, 4, 11, 2),(11, 1, 4, 12, 2),(11, 1, 4, 13, 2),(11, 1, 4, 14, 2),(11, 1, 4, 15, 2),(11, 1, 4, 16, 2),(11, 1, 4, 17, 2),(11, 1, 4, 18, 2),(11, 1, 4, 19, 2),(11, 1, 4, 20, 2),(11, 1, 4, 21, 2),(11, 1, 4, 22, 2),(11, 1, 4, 23, 2),(11, 1, 4, 24, 2),(11, 1, 4, 25, 2),(11, 1, 4, 26, 2),(11, 1, 4, 27, 2),(11, 1, 4, 28, 2),(11, 1, 4, 29, 2),(11, 1, 4, 30, 2),(11, 1, 4, 31, 2),(11, 1, 4, 32, 2),(12, 1, 4, 10, 2),(13, 1, 4, 11, 2),(14, 1, 2, 1, 2),(15, 1, 2, 1, 2),(16, 1, 2, 1, 2),(17, 1, 2, 1, 2),(18, 1, 2, 1, 2),(19, 1, 5, 10, 2),(19, 1, 5, 11, 2),(20, 1, 5, 10, 2),(21, 1, 2, 1, 2),(21, 1, 4, 2, 2),(21, 1, 4, 3, 2),(9, 1, 9, 4, 4),(9, 1, 9, 5, 4),(9, 1, 9, 6, 4),(9, 1, 9, 9, 4),(6, 1, 9, 4, 4),(6, 1, 9, 5, 4),(6, 1, 9, 6, 4),(6, 1, 9, 9, 4),(5, 1, 9, 4, 4),(5, 1, 9, 5, 4),(5, 1, 9, 6, 4),(5, 1, 9, 9, 4),(22, 1, 9, 4, 4),(22, 1, 9, 5, 4),(22, 1, 9, 9, 4),(23, 1, 9, 4, 4),(23, 1, 9, 5, 4),(23, 1, 9, 6, 4),(23, 1, 9, 9, 4),(24, 1, 9, 4, 4),(24, 1, 9, 5, 4),(24, 1, 9, 6, 4),(24, 1, 9, 9, 4),(25, 1, 9, 4, 4),(25, 1, 9, 5, 4),(25, 1, 9, 6, 4),(25, 1, 9, 9, 4),(26, 1, 9, 4, 4),(26, 1, 9, 5, 4),(26, 1, 9, 6, 4),(26, 1, 9, 9, 4),(27, 1, 9, 4, 4),(27, 1, 9, 5, 4),(27, 1, 9, 9, 4),(28, 1, 9, 4, 4),(28, 1, 9, 5, 4),(28, 1, 9, 6, 4),(28, 1, 9, 9, 4),</v>
+        <f t="array" ref="H2">_xlfn.CONCAT("INSERT INTO plumfittinginfos (plumFittingId,plumBrandId,plumGradeId,plumSizeId,plumTypeId) VALUES",(TRANSPOSE(G2:G184)&amp;","))</f>
+        <v>INSERT INTO plumfittinginfos (plumFittingId,plumBrandId,plumGradeId,plumSizeId,plumTypeId) VALUES(1, 1, 2, 1, 2),(1, 1, 4, 2, 2),(1, 1, 4, 3, 2),(1, 1, 4, 4, 2),(1, 1, 4, 5, 2),(1, 1, 4, 6, 2),(1, 1, 4, 7, 2),(1, 1, 4, 8, 2),(1, 1, 4, 9, 2),(2, 1, 2, 1, 2),(2, 1, 4, 2, 2),(2, 1, 4, 3, 2),(2, 1, 4, 4, 2),(2, 1, 4, 5, 2),(2, 1, 4, 6, 2),(2, 1, 4, 7, 2),(2, 1, 4, 8, 2),(2, 1, 4, 9, 2),(3, 1, 2, 1, 2),(3, 1, 4, 2, 2),(3, 1, 4, 3, 2),(3, 1, 4, 4, 2),(3, 1, 4, 5, 2),(3, 1, 4, 6, 2),(3, 1, 4, 7, 2),(3, 1, 4, 8, 2),(3, 1, 4, 9, 2),(4, 1, 2, 1, 2),(4, 1, 4, 2, 2),(4, 1, 4, 3, 2),(4, 1, 4, 4, 2),(4, 1, 4, 5, 2),(4, 1, 4, 6, 2),(4, 1, 4, 7, 2),(4, 1, 4, 8, 2),(4, 1, 4, 9, 2),(5, 1, 2, 1, 2),(5, 1, 4, 2, 2),(5, 1, 4, 3, 2),(5, 1, 4, 4, 2),(5, 1, 4, 5, 2),(5, 1, 4, 6, 2),(5, 1, 4, 7, 2),(5, 1, 4, 8, 2),(5, 1, 4, 9, 2),(6, 1, 2, 1, 2),(6, 1, 4, 2, 2),(6, 1, 4, 3, 2),(6, 1, 4, 4, 2),(6, 1, 4, 5, 2),(6, 1, 4, 6, 2),(6, 1, 4, 7, 2),(6, 1, 4, 8, 2),(6, 1, 4, 9, 2),(7, 1, 2, 1, 2),(7, 1, 4, 2, 2),(7, 1, 4, 3, 2),(7, 1, 4, 4, 2),(7, 1, 4, 5, 2),(7, 1, 4, 6, 2),(7, 1, 4, 7, 2),(7, 1, 4, 8, 2),(7, 1, 4, 9, 2),(8, 1, 2, 1, 2),(8, 1, 4, 2, 2),(8, 1, 4, 3, 2),(8, 1, 4, 4, 2),(8, 1, 4, 5, 2),(8, 1, 4, 6, 2),(8, 1, 4, 7, 2),(8, 1, 4, 8, 2),(8, 1, 4, 9, 2),(9, 1, 2, 1, 2),(9, 1, 4, 2, 2),(9, 1, 4, 3, 2),(9, 1, 4, 4, 2),(9, 1, 4, 5, 2),(9, 1, 4, 6, 2),(10, 1, 4, 10, 2),(10, 1, 4, 11, 2),(10, 1, 4, 12, 2),(10, 1, 4, 13, 2),(10, 1, 4, 14, 2),(10, 1, 4, 15, 2),(10, 1, 4, 16, 2),(10, 1, 4, 17, 2),(10, 1, 4, 18, 2),(10, 1, 4, 19, 2),(10, 1, 4, 20, 2),(10, 1, 4, 21, 2),(10, 1, 4, 22, 2),(10, 1, 4, 23, 2),(10, 1, 4, 24, 2),(10, 1, 4, 25, 2),(10, 1, 4, 26, 2),(10, 1, 4, 27, 2),(10, 1, 4, 28, 2),(10, 1, 4, 29, 2),(10, 1, 4, 30, 2),(10, 1, 4, 31, 2),(10, 1, 4, 32, 2),(10, 1, 4, 33, 2),(10, 1, 4, 34, 2),(10, 1, 4, 35, 2),(10, 1, 4, 36, 2),(11, 1, 4, 10, 2),(11, 1, 4, 11, 2),(11, 1, 4, 12, 2),(11, 1, 4, 13, 2),(11, 1, 4, 14, 2),(11, 1, 4, 15, 2),(11, 1, 4, 16, 2),(11, 1, 4, 17, 2),(11, 1, 4, 18, 2),(11, 1, 4, 19, 2),(11, 1, 4, 20, 2),(11, 1, 4, 21, 2),(11, 1, 4, 22, 2),(11, 1, 4, 23, 2),(11, 1, 4, 24, 2),(11, 1, 4, 25, 2),(11, 1, 4, 26, 2),(11, 1, 4, 27, 2),(11, 1, 4, 28, 2),(11, 1, 4, 29, 2),(11, 1, 4, 30, 2),(11, 1, 4, 31, 2),(11, 1, 4, 32, 2),(11, 1, 4, 33, 2),(11, 1, 4, 34, 2),(11, 1, 4, 35, 2),(11, 1, 4, 36, 2),(12, 1, 4, 10, 2),(13, 1, 4, 11, 2),(14, 1, 2, 1, 2),(15, 1, 2, 1, 2),(16, 1, 2, 1, 2),(17, 1, 2, 1, 2),(18, 1, 2, 1, 2),(19, 1, 5, 10, 2),(19, 1, 5, 11, 2),(20, 1, 5, 10, 2),(21, 1, 2, 1, 2),(21, 1, 4, 2, 2),(21, 1, 4, 3, 2),(9, 1, 9, 4, 4),(9, 1, 9, 5, 4),(9, 1, 9, 6, 4),(9, 1, 9, 9, 4),(6, 1, 9, 4, 4),(6, 1, 9, 5, 4),(6, 1, 9, 6, 4),(6, 1, 9, 9, 4),(5, 1, 9, 4, 4),(5, 1, 9, 5, 4),(5, 1, 9, 6, 4),(5, 1, 9, 9, 4),(22, 1, 9, 4, 4),(22, 1, 9, 5, 4),(22, 1, 9, 9, 4),(23, 1, 9, 4, 4),(23, 1, 9, 5, 4),(23, 1, 9, 6, 4),(23, 1, 9, 9, 4),(24, 1, 9, 4, 4),(24, 1, 9, 5, 4),(24, 1, 9, 6, 4),(24, 1, 9, 9, 4),(25, 1, 9, 4, 4),(25, 1, 9, 5, 4),(25, 1, 9, 6, 4),(25, 1, 9, 9, 4),(26, 1, 9, 4, 4),(26, 1, 9, 5, 4),(26, 1, 9, 6, 4),(26, 1, 9, 9, 4),(27, 1, 9, 4, 4),(27, 1, 9, 5, 4),(27, 1, 9, 9, 4),(28, 1, 9, 4, 4),(28, 1, 9, 5, 4),(28, 1, 9, 6, 4),(28, 1, 9, 9, 4),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4898,7 +5028,7 @@
         <v>2</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" ref="G67:G130" si="1">_xlfn.CONCAT( "(",B67,", ", C67,", ", D67,", ", E67,", ", F67,")")</f>
+        <f t="shared" ref="G67:G138" si="1">_xlfn.CONCAT( "(",B67,", ", C67,", ", D67,", ", E67,", ", F67,")")</f>
         <v>(8, 1, 4, 3, 2)</v>
       </c>
     </row>
@@ -5747,7 +5877,7 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C103">
         <v>1</v>
@@ -5756,14 +5886,14 @@
         <v>4</v>
       </c>
       <c r="E103">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="F103">
         <v>2</v>
       </c>
       <c r="G103" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 10, 2)</v>
+        <v>(10, 1, 4, 33, 2)</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -5771,7 +5901,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C104">
         <v>1</v>
@@ -5780,14 +5910,14 @@
         <v>4</v>
       </c>
       <c r="E104">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="F104">
         <v>2</v>
       </c>
       <c r="G104" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 11, 2)</v>
+        <v>(10, 1, 4, 34, 2)</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -5795,7 +5925,7 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C105">
         <v>1</v>
@@ -5804,14 +5934,14 @@
         <v>4</v>
       </c>
       <c r="E105">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="F105">
         <v>2</v>
       </c>
       <c r="G105" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 12, 2)</v>
+        <v>(10, 1, 4, 35, 2)</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -5819,7 +5949,7 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C106">
         <v>1</v>
@@ -5828,14 +5958,14 @@
         <v>4</v>
       </c>
       <c r="E106">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F106">
         <v>2</v>
       </c>
       <c r="G106" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 13, 2)</v>
+        <v>(10, 1, 4, 36, 2)</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -5852,14 +5982,14 @@
         <v>4</v>
       </c>
       <c r="E107">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F107">
         <v>2</v>
       </c>
       <c r="G107" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 14, 2)</v>
+        <v>(11, 1, 4, 10, 2)</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -5876,14 +6006,14 @@
         <v>4</v>
       </c>
       <c r="E108">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F108">
         <v>2</v>
       </c>
       <c r="G108" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 15, 2)</v>
+        <v>(11, 1, 4, 11, 2)</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -5900,14 +6030,14 @@
         <v>4</v>
       </c>
       <c r="E109">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F109">
         <v>2</v>
       </c>
       <c r="G109" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 16, 2)</v>
+        <v>(11, 1, 4, 12, 2)</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -5924,14 +6054,14 @@
         <v>4</v>
       </c>
       <c r="E110">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F110">
         <v>2</v>
       </c>
       <c r="G110" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 17, 2)</v>
+        <v>(11, 1, 4, 13, 2)</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -5948,14 +6078,14 @@
         <v>4</v>
       </c>
       <c r="E111">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F111">
         <v>2</v>
       </c>
       <c r="G111" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 18, 2)</v>
+        <v>(11, 1, 4, 14, 2)</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -5972,14 +6102,14 @@
         <v>4</v>
       </c>
       <c r="E112">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F112">
         <v>2</v>
       </c>
       <c r="G112" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 19, 2)</v>
+        <v>(11, 1, 4, 15, 2)</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -5996,14 +6126,14 @@
         <v>4</v>
       </c>
       <c r="E113">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F113">
         <v>2</v>
       </c>
       <c r="G113" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 20, 2)</v>
+        <v>(11, 1, 4, 16, 2)</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -6020,14 +6150,14 @@
         <v>4</v>
       </c>
       <c r="E114">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F114">
         <v>2</v>
       </c>
       <c r="G114" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 21, 2)</v>
+        <v>(11, 1, 4, 17, 2)</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -6044,14 +6174,14 @@
         <v>4</v>
       </c>
       <c r="E115">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F115">
         <v>2</v>
       </c>
       <c r="G115" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 22, 2)</v>
+        <v>(11, 1, 4, 18, 2)</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -6068,14 +6198,14 @@
         <v>4</v>
       </c>
       <c r="E116">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F116">
         <v>2</v>
       </c>
       <c r="G116" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 23, 2)</v>
+        <v>(11, 1, 4, 19, 2)</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -6092,14 +6222,14 @@
         <v>4</v>
       </c>
       <c r="E117">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F117">
         <v>2</v>
       </c>
       <c r="G117" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 24, 2)</v>
+        <v>(11, 1, 4, 20, 2)</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -6116,14 +6246,14 @@
         <v>4</v>
       </c>
       <c r="E118">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F118">
         <v>2</v>
       </c>
       <c r="G118" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 25, 2)</v>
+        <v>(11, 1, 4, 21, 2)</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -6140,14 +6270,14 @@
         <v>4</v>
       </c>
       <c r="E119">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F119">
         <v>2</v>
       </c>
       <c r="G119" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 26, 2)</v>
+        <v>(11, 1, 4, 22, 2)</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -6164,14 +6294,14 @@
         <v>4</v>
       </c>
       <c r="E120">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F120">
         <v>2</v>
       </c>
       <c r="G120" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 27, 2)</v>
+        <v>(11, 1, 4, 23, 2)</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -6188,14 +6318,14 @@
         <v>4</v>
       </c>
       <c r="E121">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F121">
         <v>2</v>
       </c>
       <c r="G121" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 28, 2)</v>
+        <v>(11, 1, 4, 24, 2)</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -6212,14 +6342,14 @@
         <v>4</v>
       </c>
       <c r="E122">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F122">
         <v>2</v>
       </c>
       <c r="G122" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 29, 2)</v>
+        <v>(11, 1, 4, 25, 2)</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -6236,14 +6366,14 @@
         <v>4</v>
       </c>
       <c r="E123">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F123">
         <v>2</v>
       </c>
       <c r="G123" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 30, 2)</v>
+        <v>(11, 1, 4, 26, 2)</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -6260,14 +6390,14 @@
         <v>4</v>
       </c>
       <c r="E124">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F124">
         <v>2</v>
       </c>
       <c r="G124" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 31, 2)</v>
+        <v>(11, 1, 4, 27, 2)</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -6284,14 +6414,14 @@
         <v>4</v>
       </c>
       <c r="E125">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F125">
         <v>2</v>
       </c>
       <c r="G125" t="str">
         <f t="shared" si="1"/>
-        <v>(11, 1, 4, 32, 2)</v>
+        <v>(11, 1, 4, 28, 2)</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -6299,7 +6429,7 @@
         <v>125</v>
       </c>
       <c r="B126">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C126">
         <v>1</v>
@@ -6308,14 +6438,14 @@
         <v>4</v>
       </c>
       <c r="E126">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="F126">
         <v>2</v>
       </c>
       <c r="G126" t="str">
         <f t="shared" si="1"/>
-        <v>(12, 1, 4, 10, 2)</v>
+        <v>(11, 1, 4, 29, 2)</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -6323,7 +6453,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C127">
         <v>1</v>
@@ -6332,14 +6462,14 @@
         <v>4</v>
       </c>
       <c r="E127">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="F127">
         <v>2</v>
       </c>
       <c r="G127" t="str">
         <f t="shared" si="1"/>
-        <v>(13, 1, 4, 11, 2)</v>
+        <v>(11, 1, 4, 30, 2)</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -6347,23 +6477,23 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
       <c r="D128">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E128">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="F128">
         <v>2</v>
       </c>
       <c r="G128" t="str">
         <f t="shared" si="1"/>
-        <v>(14, 1, 2, 1, 2)</v>
+        <v>(11, 1, 4, 31, 2)</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -6371,23 +6501,23 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
       <c r="D129">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E129">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="F129">
         <v>2</v>
       </c>
       <c r="G129" t="str">
         <f t="shared" si="1"/>
-        <v>(15, 1, 2, 1, 2)</v>
+        <v>(11, 1, 4, 32, 2)</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -6395,23 +6525,23 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E130">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="F130">
         <v>2</v>
       </c>
       <c r="G130" t="str">
         <f t="shared" si="1"/>
-        <v>(16, 1, 2, 1, 2)</v>
+        <v>(11, 1, 4, 33, 2)</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -6419,23 +6549,23 @@
         <v>130</v>
       </c>
       <c r="B131">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E131">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="F131">
         <v>2</v>
       </c>
       <c r="G131" t="str">
-        <f t="shared" ref="G131:G176" si="2">_xlfn.CONCAT( "(",B131,", ", C131,", ", D131,", ", E131,", ", F131,")")</f>
-        <v>(17, 1, 2, 1, 2)</v>
+        <f t="shared" si="1"/>
+        <v>(11, 1, 4, 34, 2)</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -6443,23 +6573,23 @@
         <v>131</v>
       </c>
       <c r="B132">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E132">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="F132">
         <v>2</v>
       </c>
       <c r="G132" t="str">
-        <f t="shared" si="2"/>
-        <v>(18, 1, 2, 1, 2)</v>
+        <f t="shared" si="1"/>
+        <v>(11, 1, 4, 35, 2)</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -6467,23 +6597,23 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E133">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F133">
         <v>2</v>
       </c>
       <c r="G133" t="str">
-        <f t="shared" si="2"/>
-        <v>(19, 1, 5, 10, 2)</v>
+        <f t="shared" si="1"/>
+        <v>(11, 1, 4, 36, 2)</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -6491,23 +6621,23 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
       <c r="D134">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E134">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F134">
         <v>2</v>
       </c>
       <c r="G134" t="str">
-        <f t="shared" si="2"/>
-        <v>(19, 1, 5, 11, 2)</v>
+        <f t="shared" si="1"/>
+        <v>(12, 1, 4, 10, 2)</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -6515,23 +6645,23 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C135">
         <v>1</v>
       </c>
       <c r="D135">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E135">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F135">
         <v>2</v>
       </c>
       <c r="G135" t="str">
-        <f t="shared" si="2"/>
-        <v>(20, 1, 5, 10, 2)</v>
+        <f t="shared" si="1"/>
+        <v>(13, 1, 4, 11, 2)</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -6539,7 +6669,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C136">
         <v>1</v>
@@ -6554,8 +6684,8 @@
         <v>2</v>
       </c>
       <c r="G136" t="str">
-        <f t="shared" si="2"/>
-        <v>(21, 1, 2, 1, 2)</v>
+        <f t="shared" si="1"/>
+        <v>(14, 1, 2, 1, 2)</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -6563,23 +6693,23 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C137">
         <v>1</v>
       </c>
       <c r="D137">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E137">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F137">
         <v>2</v>
       </c>
       <c r="G137" t="str">
-        <f t="shared" si="2"/>
-        <v>(21, 1, 4, 2, 2)</v>
+        <f t="shared" si="1"/>
+        <v>(15, 1, 2, 1, 2)</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -6587,23 +6717,23 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C138">
         <v>1</v>
       </c>
       <c r="D138">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E138">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F138">
         <v>2</v>
       </c>
       <c r="G138" t="str">
-        <f t="shared" si="2"/>
-        <v>(21, 1, 4, 3, 2)</v>
+        <f t="shared" si="1"/>
+        <v>(16, 1, 2, 1, 2)</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -6611,23 +6741,23 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C139">
         <v>1</v>
       </c>
       <c r="D139">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E139">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F139">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G139" t="str">
-        <f t="shared" si="2"/>
-        <v>(9, 1, 9, 4, 4)</v>
+        <f t="shared" ref="G139:G184" si="2">_xlfn.CONCAT( "(",B139,", ", C139,", ", D139,", ", E139,", ", F139,")")</f>
+        <v>(17, 1, 2, 1, 2)</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
@@ -6635,23 +6765,23 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C140">
         <v>1</v>
       </c>
       <c r="D140">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E140">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F140">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G140" t="str">
         <f t="shared" si="2"/>
-        <v>(9, 1, 9, 5, 4)</v>
+        <v>(18, 1, 2, 1, 2)</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -6659,23 +6789,23 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C141">
         <v>1</v>
       </c>
       <c r="D141">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E141">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F141">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G141" t="str">
         <f t="shared" si="2"/>
-        <v>(9, 1, 9, 6, 4)</v>
+        <v>(19, 1, 5, 10, 2)</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -6683,23 +6813,23 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C142">
         <v>1</v>
       </c>
       <c r="D142">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E142">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F142">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G142" t="str">
         <f t="shared" si="2"/>
-        <v>(9, 1, 9, 9, 4)</v>
+        <v>(19, 1, 5, 11, 2)</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -6707,23 +6837,23 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C143">
         <v>1</v>
       </c>
       <c r="D143">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E143">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F143">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G143" t="str">
         <f t="shared" si="2"/>
-        <v>(6, 1, 9, 4, 4)</v>
+        <v>(20, 1, 5, 10, 2)</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
@@ -6731,23 +6861,23 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C144">
         <v>1</v>
       </c>
       <c r="D144">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E144">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F144">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G144" t="str">
         <f t="shared" si="2"/>
-        <v>(6, 1, 9, 5, 4)</v>
+        <v>(21, 1, 2, 1, 2)</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
@@ -6755,23 +6885,23 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C145">
         <v>1</v>
       </c>
       <c r="D145">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E145">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F145">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G145" t="str">
         <f t="shared" si="2"/>
-        <v>(6, 1, 9, 6, 4)</v>
+        <v>(21, 1, 4, 2, 2)</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -6779,23 +6909,23 @@
         <v>145</v>
       </c>
       <c r="B146">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C146">
         <v>1</v>
       </c>
       <c r="D146">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E146">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F146">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G146" t="str">
         <f t="shared" si="2"/>
-        <v>(6, 1, 9, 9, 4)</v>
+        <v>(21, 1, 4, 3, 2)</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
@@ -6803,7 +6933,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C147">
         <v>1</v>
@@ -6819,7 +6949,7 @@
       </c>
       <c r="G147" t="str">
         <f t="shared" si="2"/>
-        <v>(5, 1, 9, 4, 4)</v>
+        <v>(9, 1, 9, 4, 4)</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -6827,7 +6957,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C148">
         <v>1</v>
@@ -6843,7 +6973,7 @@
       </c>
       <c r="G148" t="str">
         <f t="shared" si="2"/>
-        <v>(5, 1, 9, 5, 4)</v>
+        <v>(9, 1, 9, 5, 4)</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -6851,7 +6981,7 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C149">
         <v>1</v>
@@ -6867,7 +6997,7 @@
       </c>
       <c r="G149" t="str">
         <f t="shared" si="2"/>
-        <v>(5, 1, 9, 6, 4)</v>
+        <v>(9, 1, 9, 6, 4)</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
@@ -6875,7 +7005,7 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C150">
         <v>1</v>
@@ -6891,7 +7021,7 @@
       </c>
       <c r="G150" t="str">
         <f t="shared" si="2"/>
-        <v>(5, 1, 9, 9, 4)</v>
+        <v>(9, 1, 9, 9, 4)</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
@@ -6899,7 +7029,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C151">
         <v>1</v>
@@ -6915,7 +7045,7 @@
       </c>
       <c r="G151" t="str">
         <f t="shared" si="2"/>
-        <v>(22, 1, 9, 4, 4)</v>
+        <v>(6, 1, 9, 4, 4)</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
@@ -6923,7 +7053,7 @@
         <v>151</v>
       </c>
       <c r="B152">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C152">
         <v>1</v>
@@ -6939,7 +7069,7 @@
       </c>
       <c r="G152" t="str">
         <f t="shared" si="2"/>
-        <v>(22, 1, 9, 5, 4)</v>
+        <v>(6, 1, 9, 5, 4)</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -6947,7 +7077,7 @@
         <v>152</v>
       </c>
       <c r="B153">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C153">
         <v>1</v>
@@ -6956,14 +7086,14 @@
         <v>9</v>
       </c>
       <c r="E153">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F153">
         <v>4</v>
       </c>
       <c r="G153" t="str">
         <f t="shared" si="2"/>
-        <v>(22, 1, 9, 9, 4)</v>
+        <v>(6, 1, 9, 6, 4)</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
@@ -6971,7 +7101,7 @@
         <v>153</v>
       </c>
       <c r="B154">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C154">
         <v>1</v>
@@ -6980,14 +7110,14 @@
         <v>9</v>
       </c>
       <c r="E154">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F154">
         <v>4</v>
       </c>
       <c r="G154" t="str">
         <f t="shared" si="2"/>
-        <v>(23, 1, 9, 4, 4)</v>
+        <v>(6, 1, 9, 9, 4)</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
@@ -6995,7 +7125,7 @@
         <v>154</v>
       </c>
       <c r="B155">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C155">
         <v>1</v>
@@ -7004,14 +7134,14 @@
         <v>9</v>
       </c>
       <c r="E155">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F155">
         <v>4</v>
       </c>
       <c r="G155" t="str">
         <f t="shared" si="2"/>
-        <v>(23, 1, 9, 5, 4)</v>
+        <v>(5, 1, 9, 4, 4)</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -7019,7 +7149,7 @@
         <v>155</v>
       </c>
       <c r="B156">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C156">
         <v>1</v>
@@ -7028,14 +7158,14 @@
         <v>9</v>
       </c>
       <c r="E156">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F156">
         <v>4</v>
       </c>
       <c r="G156" t="str">
         <f t="shared" si="2"/>
-        <v>(23, 1, 9, 6, 4)</v>
+        <v>(5, 1, 9, 5, 4)</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -7043,7 +7173,7 @@
         <v>156</v>
       </c>
       <c r="B157">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C157">
         <v>1</v>
@@ -7052,14 +7182,14 @@
         <v>9</v>
       </c>
       <c r="E157">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F157">
         <v>4</v>
       </c>
       <c r="G157" t="str">
         <f t="shared" si="2"/>
-        <v>(23, 1, 9, 9, 4)</v>
+        <v>(5, 1, 9, 6, 4)</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
@@ -7067,7 +7197,7 @@
         <v>157</v>
       </c>
       <c r="B158">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C158">
         <v>1</v>
@@ -7076,14 +7206,14 @@
         <v>9</v>
       </c>
       <c r="E158">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F158">
         <v>4</v>
       </c>
       <c r="G158" t="str">
         <f t="shared" si="2"/>
-        <v>(24, 1, 9, 4, 4)</v>
+        <v>(5, 1, 9, 9, 4)</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
@@ -7091,7 +7221,7 @@
         <v>158</v>
       </c>
       <c r="B159">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C159">
         <v>1</v>
@@ -7100,14 +7230,14 @@
         <v>9</v>
       </c>
       <c r="E159">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F159">
         <v>4</v>
       </c>
       <c r="G159" t="str">
         <f t="shared" si="2"/>
-        <v>(24, 1, 9, 5, 4)</v>
+        <v>(22, 1, 9, 4, 4)</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
@@ -7115,7 +7245,7 @@
         <v>159</v>
       </c>
       <c r="B160">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C160">
         <v>1</v>
@@ -7124,14 +7254,14 @@
         <v>9</v>
       </c>
       <c r="E160">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F160">
         <v>4</v>
       </c>
       <c r="G160" t="str">
         <f t="shared" si="2"/>
-        <v>(24, 1, 9, 6, 4)</v>
+        <v>(22, 1, 9, 5, 4)</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -7139,7 +7269,7 @@
         <v>160</v>
       </c>
       <c r="B161">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C161">
         <v>1</v>
@@ -7155,7 +7285,7 @@
       </c>
       <c r="G161" t="str">
         <f t="shared" si="2"/>
-        <v>(24, 1, 9, 9, 4)</v>
+        <v>(22, 1, 9, 9, 4)</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
@@ -7163,7 +7293,7 @@
         <v>161</v>
       </c>
       <c r="B162">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C162">
         <v>1</v>
@@ -7179,7 +7309,7 @@
       </c>
       <c r="G162" t="str">
         <f t="shared" si="2"/>
-        <v>(25, 1, 9, 4, 4)</v>
+        <v>(23, 1, 9, 4, 4)</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
@@ -7187,7 +7317,7 @@
         <v>162</v>
       </c>
       <c r="B163">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C163">
         <v>1</v>
@@ -7203,7 +7333,7 @@
       </c>
       <c r="G163" t="str">
         <f t="shared" si="2"/>
-        <v>(25, 1, 9, 5, 4)</v>
+        <v>(23, 1, 9, 5, 4)</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -7211,7 +7341,7 @@
         <v>163</v>
       </c>
       <c r="B164">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C164">
         <v>1</v>
@@ -7227,7 +7357,7 @@
       </c>
       <c r="G164" t="str">
         <f t="shared" si="2"/>
-        <v>(25, 1, 9, 6, 4)</v>
+        <v>(23, 1, 9, 6, 4)</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
@@ -7235,7 +7365,7 @@
         <v>164</v>
       </c>
       <c r="B165">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C165">
         <v>1</v>
@@ -7251,7 +7381,7 @@
       </c>
       <c r="G165" t="str">
         <f t="shared" si="2"/>
-        <v>(25, 1, 9, 9, 4)</v>
+        <v>(23, 1, 9, 9, 4)</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
@@ -7259,7 +7389,7 @@
         <v>165</v>
       </c>
       <c r="B166">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C166">
         <v>1</v>
@@ -7275,7 +7405,7 @@
       </c>
       <c r="G166" t="str">
         <f t="shared" si="2"/>
-        <v>(26, 1, 9, 4, 4)</v>
+        <v>(24, 1, 9, 4, 4)</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
@@ -7283,7 +7413,7 @@
         <v>166</v>
       </c>
       <c r="B167">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C167">
         <v>1</v>
@@ -7299,7 +7429,7 @@
       </c>
       <c r="G167" t="str">
         <f t="shared" si="2"/>
-        <v>(26, 1, 9, 5, 4)</v>
+        <v>(24, 1, 9, 5, 4)</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
@@ -7307,7 +7437,7 @@
         <v>167</v>
       </c>
       <c r="B168">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C168">
         <v>1</v>
@@ -7323,7 +7453,7 @@
       </c>
       <c r="G168" t="str">
         <f t="shared" si="2"/>
-        <v>(26, 1, 9, 6, 4)</v>
+        <v>(24, 1, 9, 6, 4)</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
@@ -7331,7 +7461,7 @@
         <v>168</v>
       </c>
       <c r="B169">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C169">
         <v>1</v>
@@ -7347,7 +7477,7 @@
       </c>
       <c r="G169" t="str">
         <f t="shared" si="2"/>
-        <v>(26, 1, 9, 9, 4)</v>
+        <v>(24, 1, 9, 9, 4)</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
@@ -7355,7 +7485,7 @@
         <v>169</v>
       </c>
       <c r="B170">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C170">
         <v>1</v>
@@ -7371,7 +7501,7 @@
       </c>
       <c r="G170" t="str">
         <f t="shared" si="2"/>
-        <v>(27, 1, 9, 4, 4)</v>
+        <v>(25, 1, 9, 4, 4)</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
@@ -7379,7 +7509,7 @@
         <v>170</v>
       </c>
       <c r="B171">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C171">
         <v>1</v>
@@ -7395,7 +7525,7 @@
       </c>
       <c r="G171" t="str">
         <f t="shared" si="2"/>
-        <v>(27, 1, 9, 5, 4)</v>
+        <v>(25, 1, 9, 5, 4)</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
@@ -7403,7 +7533,7 @@
         <v>171</v>
       </c>
       <c r="B172">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C172">
         <v>1</v>
@@ -7412,14 +7542,14 @@
         <v>9</v>
       </c>
       <c r="E172">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F172">
         <v>4</v>
       </c>
       <c r="G172" t="str">
         <f t="shared" si="2"/>
-        <v>(27, 1, 9, 9, 4)</v>
+        <v>(25, 1, 9, 6, 4)</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
@@ -7427,7 +7557,7 @@
         <v>172</v>
       </c>
       <c r="B173">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C173">
         <v>1</v>
@@ -7436,14 +7566,14 @@
         <v>9</v>
       </c>
       <c r="E173">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F173">
         <v>4</v>
       </c>
       <c r="G173" t="str">
         <f t="shared" si="2"/>
-        <v>(28, 1, 9, 4, 4)</v>
+        <v>(25, 1, 9, 9, 4)</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
@@ -7451,7 +7581,7 @@
         <v>173</v>
       </c>
       <c r="B174">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C174">
         <v>1</v>
@@ -7460,14 +7590,14 @@
         <v>9</v>
       </c>
       <c r="E174">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F174">
         <v>4</v>
       </c>
       <c r="G174" t="str">
         <f t="shared" si="2"/>
-        <v>(28, 1, 9, 5, 4)</v>
+        <v>(26, 1, 9, 4, 4)</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
@@ -7475,7 +7605,7 @@
         <v>174</v>
       </c>
       <c r="B175">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C175">
         <v>1</v>
@@ -7484,14 +7614,14 @@
         <v>9</v>
       </c>
       <c r="E175">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F175">
         <v>4</v>
       </c>
       <c r="G175" t="str">
         <f t="shared" si="2"/>
-        <v>(28, 1, 9, 6, 4)</v>
+        <v>(26, 1, 9, 5, 4)</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
@@ -7499,7 +7629,7 @@
         <v>175</v>
       </c>
       <c r="B176">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C176">
         <v>1</v>
@@ -7508,12 +7638,204 @@
         <v>9</v>
       </c>
       <c r="E176">
+        <v>6</v>
+      </c>
+      <c r="F176">
+        <v>4</v>
+      </c>
+      <c r="G176" t="str">
+        <f t="shared" si="2"/>
+        <v>(26, 1, 9, 6, 4)</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>176</v>
+      </c>
+      <c r="B177">
+        <v>26</v>
+      </c>
+      <c r="C177">
+        <v>1</v>
+      </c>
+      <c r="D177">
         <v>9</v>
       </c>
-      <c r="F176">
-        <v>4</v>
-      </c>
-      <c r="G176" t="str">
+      <c r="E177">
+        <v>9</v>
+      </c>
+      <c r="F177">
+        <v>4</v>
+      </c>
+      <c r="G177" t="str">
+        <f t="shared" si="2"/>
+        <v>(26, 1, 9, 9, 4)</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>177</v>
+      </c>
+      <c r="B178">
+        <v>27</v>
+      </c>
+      <c r="C178">
+        <v>1</v>
+      </c>
+      <c r="D178">
+        <v>9</v>
+      </c>
+      <c r="E178">
+        <v>4</v>
+      </c>
+      <c r="F178">
+        <v>4</v>
+      </c>
+      <c r="G178" t="str">
+        <f t="shared" si="2"/>
+        <v>(27, 1, 9, 4, 4)</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>178</v>
+      </c>
+      <c r="B179">
+        <v>27</v>
+      </c>
+      <c r="C179">
+        <v>1</v>
+      </c>
+      <c r="D179">
+        <v>9</v>
+      </c>
+      <c r="E179">
+        <v>5</v>
+      </c>
+      <c r="F179">
+        <v>4</v>
+      </c>
+      <c r="G179" t="str">
+        <f t="shared" si="2"/>
+        <v>(27, 1, 9, 5, 4)</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>179</v>
+      </c>
+      <c r="B180">
+        <v>27</v>
+      </c>
+      <c r="C180">
+        <v>1</v>
+      </c>
+      <c r="D180">
+        <v>9</v>
+      </c>
+      <c r="E180">
+        <v>9</v>
+      </c>
+      <c r="F180">
+        <v>4</v>
+      </c>
+      <c r="G180" t="str">
+        <f t="shared" si="2"/>
+        <v>(27, 1, 9, 9, 4)</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>180</v>
+      </c>
+      <c r="B181">
+        <v>28</v>
+      </c>
+      <c r="C181">
+        <v>1</v>
+      </c>
+      <c r="D181">
+        <v>9</v>
+      </c>
+      <c r="E181">
+        <v>4</v>
+      </c>
+      <c r="F181">
+        <v>4</v>
+      </c>
+      <c r="G181" t="str">
+        <f t="shared" si="2"/>
+        <v>(28, 1, 9, 4, 4)</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>181</v>
+      </c>
+      <c r="B182">
+        <v>28</v>
+      </c>
+      <c r="C182">
+        <v>1</v>
+      </c>
+      <c r="D182">
+        <v>9</v>
+      </c>
+      <c r="E182">
+        <v>5</v>
+      </c>
+      <c r="F182">
+        <v>4</v>
+      </c>
+      <c r="G182" t="str">
+        <f t="shared" si="2"/>
+        <v>(28, 1, 9, 5, 4)</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>182</v>
+      </c>
+      <c r="B183">
+        <v>28</v>
+      </c>
+      <c r="C183">
+        <v>1</v>
+      </c>
+      <c r="D183">
+        <v>9</v>
+      </c>
+      <c r="E183">
+        <v>6</v>
+      </c>
+      <c r="F183">
+        <v>4</v>
+      </c>
+      <c r="G183" t="str">
+        <f t="shared" si="2"/>
+        <v>(28, 1, 9, 6, 4)</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>183</v>
+      </c>
+      <c r="B184">
+        <v>28</v>
+      </c>
+      <c r="C184">
+        <v>1</v>
+      </c>
+      <c r="D184">
+        <v>9</v>
+      </c>
+      <c r="E184">
+        <v>9</v>
+      </c>
+      <c r="F184">
+        <v>4</v>
+      </c>
+      <c r="G184" t="str">
         <f t="shared" si="2"/>
         <v>(28, 1, 9, 9, 4)</v>
       </c>
@@ -7591,7 +7913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD72405-4BAA-4BE0-9E9A-35EF3BE8961C}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>

</xml_diff>